<commit_message>
Corrections for the export
It was exporting wrong the PPG column, now it is correct
</commit_message>
<xml_diff>
--- a/seletivo-lattes/seletivo_lattes.xlsx
+++ b/seletivo-lattes/seletivo_lattes.xlsx
@@ -14,48 +14,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
-  <si>
-    <t>nome</t>
-  </si>
-  <si>
-    <t>cv_lattes</t>
-  </si>
-  <si>
-    <t>PPG</t>
-  </si>
-  <si>
-    <t>ultima_atualizacao</t>
-  </si>
-  <si>
-    <t>endereco_prof</t>
-  </si>
-  <si>
-    <t>ano_ultima_formacao</t>
-  </si>
-  <si>
-    <t>formacao_titulo</t>
-  </si>
-  <si>
-    <t>formacao_ies</t>
-  </si>
-  <si>
-    <t>ultimo_vinculo_ies</t>
-  </si>
-  <si>
-    <t>prod_artigos_completos</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+  <si>
+    <t>http://lattes.cnpq.br/3269118444404338</t>
+  </si>
+  <si>
+    <t>http://lattes.cnpq.br/2281909649311607</t>
+  </si>
+  <si>
+    <t>GEAS</t>
+  </si>
+  <si>
+    <t>PPGA-D</t>
   </si>
   <si>
     <t>Patricia Storópoli Tzortzis</t>
   </si>
   <si>
     <t>José Eduardo Storopoli</t>
-  </si>
-  <si>
-    <t>http://lattes.cnpq.br/3269118444404338</t>
-  </si>
-  <si>
-    <t>GEAS</t>
   </si>
   <si>
     <t>24/04/2017</t>
@@ -466,96 +442,96 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="1">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="1">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="1">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="1">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="1">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="1">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="1">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="1">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="1">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="1">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="G2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="H2" t="s">
         <v>14</v>
       </c>
-      <c r="E2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" t="s">
-        <v>22</v>
-      </c>
       <c r="I2" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="J2">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="G3" t="s">
         <v>13</v>
       </c>
-      <c r="D3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" t="s">
-        <v>21</v>
-      </c>
       <c r="H3" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="I3" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="J3">
         <v>17</v>
@@ -563,8 +539,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Inserção de Colnames no DF final
inseri os seguintes rótulos como cabeçalhos das 10 colunas do DF que é exportado: link_lattes','PPG',                     'nome','ultima_atualizacao',                  'endereco_prof','ano_ultima_formacao', 'formacao_titulo','ultimo_vinculo_ies','prod_artigos_completos']
</commit_message>
<xml_diff>
--- a/seletivo-lattes/seletivo_lattes.xlsx
+++ b/seletivo-lattes/seletivo_lattes.xlsx
@@ -14,7 +14,37 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+  <si>
+    <t>link_lattes</t>
+  </si>
+  <si>
+    <t>PPG</t>
+  </si>
+  <si>
+    <t>nome</t>
+  </si>
+  <si>
+    <t>ultima_atualizacao</t>
+  </si>
+  <si>
+    <t>endereco_prof</t>
+  </si>
+  <si>
+    <t>ano_ultima_formacao</t>
+  </si>
+  <si>
+    <t>formacao_titulo</t>
+  </si>
+  <si>
+    <t>formacao_ies</t>
+  </si>
+  <si>
+    <t>ultimo_vinculo_ies</t>
+  </si>
+  <si>
+    <t>prod_artigos_completos</t>
+  </si>
   <si>
     <t>http://lattes.cnpq.br/3269118444404338</t>
   </si>
@@ -442,64 +472,64 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="1">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="2" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="F2" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="G2" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="H2" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="I2" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="J2">
         <v>1</v>
@@ -507,31 +537,31 @@
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="2" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="F3" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="G3" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="H3" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="I3" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="J3">
         <v>17</v>

</xml_diff>